<commit_message>
avoid dependencies on reactions with 0 net stoichiometry for a species; convert dependencies into more compact and faster list of tuples; add stub code for dependencies on species in a continuous submodels
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
+++ b/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2760" windowWidth="28700" windowHeight="13960" tabRatio="993" firstSheet="8" activeTab="16"/>
-    <workbookView xWindow="-26740" yWindow="780" windowWidth="25840" windowHeight="13800" tabRatio="500" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="2760" windowWidth="28700" windowHeight="13960" tabRatio="993" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="-26740" yWindow="780" windowWidth="25840" windowHeight="13800" tabRatio="500" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -53,40 +53,40 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$K$9</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="16">[2]Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="21">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="246">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -821,6 +821,24 @@
   </si>
   <si>
     <t>k_4 * e[c] * e[c] * f[c]</t>
+  </si>
+  <si>
+    <t>reaction_6</t>
+  </si>
+  <si>
+    <t>reaction_name_6</t>
+  </si>
+  <si>
+    <t>[c]: f ==&gt;</t>
+  </si>
+  <si>
+    <t>reaction_6-forward</t>
+  </si>
+  <si>
+    <t>k_6</t>
+  </si>
+  <si>
+    <t>k_6 * f[c]</t>
   </si>
 </sst>
 </file>
@@ -926,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -988,6 +1006,9 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1038,7 +1059,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Species types"/>
+      <sheetName val="Parameters"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1064,7 +1085,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Parameters"/>
+      <sheetName val="References"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1077,7 +1098,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="References"/>
+      <sheetName val="Species types"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1760,7 +1781,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM8"/>
+  <dimension ref="A1:AMM9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -1769,8 +1790,8 @@
       <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
       <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1796,11 +1817,11 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
@@ -3993,6 +4014,26 @@
         <v>119</v>
       </c>
     </row>
+    <row r="9" spans="1:1027" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:D7"/>
   <mergeCells count="1">
@@ -4005,16 +4046,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:F8"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="F3" sqref="F3:F8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4035,7 +4076,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>29</v>
       </c>
@@ -4073,7 +4114,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>129</v>
       </c>
@@ -4090,7 +4131,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>131</v>
       </c>
@@ -4107,7 +4148,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>132</v>
       </c>
@@ -4124,7 +4165,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>133</v>
       </c>
@@ -4156,6 +4197,25 @@
         <v>231</v>
       </c>
       <c r="G7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4376,23 +4436,23 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:A10"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="44.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="34.5" style="16" customWidth="1"/>
     <col min="3" max="4" width="9.1640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="8.83203125" style="16" customWidth="1"/>
     <col min="12" max="1026" width="8.83203125" style="5" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="5" customWidth="1"/>
@@ -4404,7 +4464,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>29</v>
       </c>
@@ -4439,7 +4499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>143</v>
       </c>
@@ -4531,6 +4591,20 @@
       </c>
       <c r="F10" s="16" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4628,26 +4702,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="26" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="Q2" s="27" t="s">
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="Q2" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="R2" s="24"/>
-      <c r="S2" s="27" t="s">
+      <c r="R2" s="25"/>
+      <c r="S2" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="T2" s="24"/>
+      <c r="T2" s="25"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -4939,10 +5013,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -5535,19 +5609,19 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
@@ -7738,15 +7812,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="1:14" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="C2" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">

</xml_diff>

<commit_message>
draft NRM code that updates just reactions that depend on species changed by the reaction that just executed, or other submodels
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
+++ b/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2760" windowWidth="28700" windowHeight="13960" tabRatio="993" firstSheet="8" activeTab="12"/>
-    <workbookView xWindow="-26740" yWindow="780" windowWidth="25840" windowHeight="13800" tabRatio="500" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2760" windowWidth="28700" windowHeight="13960" tabRatio="993" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="-26740" yWindow="780" windowWidth="25840" windowHeight="13800" tabRatio="500" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="245">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -410,9 +410,6 @@
   </si>
   <si>
     <t>!Species</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>!!ObjTables type='Data' id='Observable' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
@@ -1660,7 +1657,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1671,7 +1668,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>73</v>
@@ -1726,7 +1723,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1737,7 +1734,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>73</v>
@@ -1760,10 +1757,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>108</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>83</v>
@@ -1790,7 +1787,7 @@
       <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
       <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1807,7 +1804,7 @@
   <sheetData>
     <row r="1" spans="1:1027" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:1027" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1818,7 +1815,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
@@ -2849,22 +2846,22 @@
         <v>30</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>73</v>
@@ -3900,22 +3897,22 @@
     </row>
     <row r="4" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>118</v>
-      </c>
       <c r="C4" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -3924,22 +3921,22 @@
     </row>
     <row r="5" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>121</v>
-      </c>
       <c r="C5" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3948,22 +3945,22 @@
     </row>
     <row r="6" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="C6" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -3972,22 +3969,22 @@
     </row>
     <row r="7" spans="1:1027" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="C7" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -3996,42 +3993,42 @@
     </row>
     <row r="8" spans="1:1027" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>219</v>
-      </c>
       <c r="C8" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:1027" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="E9" s="12">
         <v>0</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4048,7 +4045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -4073,7 +4070,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
@@ -4084,16 +4081,16 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>128</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>73</v>
@@ -4116,107 +4113,107 @@
     </row>
     <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="F3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4245,7 +4242,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4256,19 +4253,19 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F2" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>136</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>42</v>
@@ -4314,7 +4311,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28" x14ac:dyDescent="0.2">
@@ -4325,13 +4322,13 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>42</v>
@@ -4386,7 +4383,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
@@ -4397,7 +4394,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>102</v>
@@ -4438,7 +4435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -4461,7 +4458,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
@@ -4478,7 +4475,7 @@
         <v>89</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>73</v>
@@ -4501,10 +4498,10 @@
     </row>
     <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>144</v>
       </c>
       <c r="D3" s="16">
         <v>0.3</v>
@@ -4513,7 +4510,7 @@
         <v>85</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4524,78 +4521,78 @@
         <v>1100</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" s="6">
         <v>6.02214075862E+23</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" s="16">
         <v>1</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="16">
         <v>1</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -4604,7 +4601,7 @@
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -4636,7 +4633,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4647,7 +4644,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>73</v>
@@ -4698,16 +4695,16 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G2" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
@@ -4715,11 +4712,11 @@
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="Q2" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R2" s="25"/>
       <c r="S2" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T2" s="25"/>
     </row>
@@ -4734,7 +4731,7 @@
         <v>89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>73</v>
@@ -4743,10 +4740,10 @@
         <v>95</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>55</v>
@@ -4758,19 +4755,19 @@
         <v>64</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>30</v>
@@ -4837,7 +4834,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4845,7 +4842,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4947,7 +4944,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4958,7 +4955,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
@@ -5009,12 +5006,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H2" s="25"/>
     </row>
@@ -5029,7 +5026,7 @@
         <v>89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>73</v>
@@ -5056,10 +5053,10 @@
         <v>52</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5133,7 +5130,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -5144,46 +5141,46 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>171</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>172</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>95</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>180</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>181</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>42</v>
@@ -5219,7 +5216,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -5230,28 +5227,28 @@
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>189</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>42</v>
@@ -5285,7 +5282,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -5299,25 +5296,25 @@
         <v>95</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>196</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>197</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>42</v>
@@ -5335,10 +5332,10 @@
         <v>52</v>
       </c>
       <c r="P2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q2" s="14" t="s">
         <v>166</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -5553,13 +5550,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -7868,10 +7865,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G4" s="16">
         <v>1</v>
@@ -7886,10 +7883,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G5" s="16">
         <v>2</v>
@@ -7922,10 +7919,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G7" s="16">
         <v>4</v>
@@ -7958,10 +7955,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="16">
         <v>6</v>
@@ -8046,10 +8043,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>75</v>
@@ -8060,10 +8057,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>75</v>
@@ -8074,7 +8071,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>75</v>
@@ -8088,10 +8085,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>75</v>
@@ -8102,7 +8099,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>80</v>
@@ -8116,10 +8113,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>75</v>
@@ -8149,8 +8146,8 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8177,7 +8174,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>29</v>
       </c>
@@ -8217,104 +8214,122 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E3" s="20">
-        <v>1.4799999999999999E-4</v>
+        <v>1000000</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E4" s="20">
-        <v>2.0000000000000001E-4</v>
+        <v>1000000</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E5" s="20">
-        <v>5.0000000000000001E-4</v>
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E6" s="20">
-        <v>5.0000000000000001E-4</v>
+        <v>1000000</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E7" s="20">
-        <v>1E-3</v>
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E8" s="20">
-        <v>2E-3</v>
+        <v>1000000</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish building the core NRM in WC Sim; make reactions execute at once / second, on average
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
+++ b/tests/submodels/fixtures/test_next_reaction_method_submodel.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2760" windowWidth="28700" windowHeight="13960" tabRatio="993" firstSheet="8" activeTab="16"/>
-    <workbookView xWindow="-26740" yWindow="780" windowWidth="25840" windowHeight="13800" tabRatio="500" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="3520" yWindow="500" windowWidth="31280" windowHeight="14680" tabRatio="500" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="-28420" yWindow="1700" windowWidth="28160" windowHeight="16880" tabRatio="500" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1364,11 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1639,14 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1703,13 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1781,15 +1766,9 @@
   <dimension ref="A1:AMM9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4046,14 +4025,9 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
-    </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4226,12 +4200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4292,13 +4261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4360,12 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4436,10 +4394,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -4539,8 +4494,8 @@
       <c r="A6" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="D6" s="16">
-        <v>1</v>
+      <c r="D6" s="6">
+        <v>1E-3</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>231</v>
@@ -4550,8 +4505,8 @@
       <c r="A7" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="D7" s="16">
-        <v>1</v>
+      <c r="D7" s="6">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>232</v>
@@ -4561,8 +4516,8 @@
       <c r="A8" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="D8" s="16">
-        <v>1</v>
+      <c r="D8" s="6">
+        <v>1E-3</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>231</v>
@@ -4572,8 +4527,8 @@
       <c r="A9" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="D9" s="16">
-        <v>1</v>
+      <c r="D9" s="6">
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>233</v>
@@ -4596,8 +4551,8 @@
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="22">
-        <v>1</v>
+      <c r="D11" s="6">
+        <v>1E-3</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -4615,13 +4570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4679,12 +4628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:V1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4806,14 +4750,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4926,12 +4866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="A2:F5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4988,12 +4923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5108,12 +5038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5200,12 +5125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5266,12 +5186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5347,12 +5262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5418,12 +5329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5492,16 +5399,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5569,16 +5470,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7777,16 +7672,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A19:A21"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7987,14 +7876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A21" sqref="A19:A21"/>
-      <selection pane="topRight" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A19:A21"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8139,16 +8022,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E8"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8223,7 +8100,7 @@
         <v>82</v>
       </c>
       <c r="E3" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="16">
         <v>0</v>
@@ -8243,7 +8120,7 @@
         <v>82</v>
       </c>
       <c r="E4" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F4" s="22">
         <v>0</v>
@@ -8263,7 +8140,7 @@
         <v>82</v>
       </c>
       <c r="E5" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="22">
         <v>0</v>
@@ -8283,7 +8160,7 @@
         <v>82</v>
       </c>
       <c r="E6" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="22">
         <v>0</v>
@@ -8303,7 +8180,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="22">
         <v>0</v>
@@ -8323,7 +8200,7 @@
         <v>82</v>
       </c>
       <c r="E8" s="20">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="F8" s="22">
         <v>0</v>

</xml_diff>